<commit_message>
Connect to database and initial analysis.
</commit_message>
<xml_diff>
--- a/presentation/Planning.xlsx
+++ b/presentation/Planning.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PyCharm\AmazonProduct\presentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\PyCharm\product-review\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2964"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2964" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
     <sheet name="Performance" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Documents</t>
   </si>
@@ -67,6 +68,24 @@
   </si>
   <si>
     <t>Join dataset: only get metadata of those having a review in the review dataset.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>metadata</t>
+  </si>
+  <si>
+    <t>product reviews</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>price overall</t>
   </si>
 </sst>
 </file>
@@ -74,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -118,8 +137,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -510,52 +529,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
         <v>9420571</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>2222</v>
       </c>
-      <c r="C2" s="1">
-        <f>B2/60</f>
+      <c r="D2" s="1">
+        <f>C2/60</f>
         <v>37.033333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>19815270</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>17615000</v>
+      </c>
+      <c r="C3" s="1">
         <v>5770</v>
       </c>
-      <c r="C3" s="1">
-        <f>B3/60</f>
+      <c r="D3" s="1">
+        <f>C3/60</f>
         <v>96.166666666666671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>16964379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>2952306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>2467052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>